<commit_message>
Added the new data, fixed the final plots and data, and changed to Chuck's Lead AA C Altitude Deviation Example.
</commit_message>
<xml_diff>
--- a/Scoring_SHADOW/Scenario_C.xlsx
+++ b/Scoring_SHADOW/Scenario_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coolhomie1987/Documents/MATLAB/TPS/TMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683CCF5B-9924-2549-BE3E-508324685D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E646101-B3ED-9C4E-BF09-F665774B0B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{86F4C2D8-6DB1-B24C-A877-DA67AA4DB40E}"/>
+    <workbookView xWindow="1740" yWindow="900" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{86F4C2D8-6DB1-B24C-A877-DA67AA4DB40E}"/>
   </bookViews>
   <sheets>
     <sheet name="HH" sheetId="1" r:id="rId1"/>
@@ -5863,7 +5863,7 @@
   <dimension ref="A1:BS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BQ13" sqref="BQ13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6721,13 +6721,13 @@
         <v>5</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>55.900501761614102</v>
       </c>
       <c r="L5">
         <v>0</v>

</xml_diff>